<commit_message>
#Không import được hàng hóa từ file excel #Import được hàng hóa nhưng trên danh sách hàng hóa không tính ra được trọng lượng và kích thước của từng mặt hàng #fix lỗi
</commit_message>
<xml_diff>
--- a/Document/4.Test/1.UpToNow_Loi_DeXuatSua.xlsx
+++ b/Document/4.Test/1.UpToNow_Loi_DeXuatSua.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC524A57-945A-424B-8B09-CDEB702D2E44}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84F6F63-3576-464B-8ABE-235A2493E5E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loi" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
   <si>
     <t>TT</t>
   </si>
@@ -387,9 +387,6 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -402,6 +399,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -691,24 +691,24 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" customWidth="1"/>
-    <col min="5" max="5" width="41.1796875" customWidth="1"/>
-    <col min="6" max="6" width="21.1796875" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" customWidth="1"/>
-    <col min="8" max="9" width="12.26953125" customWidth="1"/>
-    <col min="10" max="10" width="9.26953125" customWidth="1"/>
-    <col min="11" max="11" width="38.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="41.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" customWidth="1"/>
+    <col min="11" max="11" width="38.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -743,7 +743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -776,7 +776,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -809,7 +809,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -842,7 +842,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -875,69 +875,69 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="18">
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
         <v>5</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="20">
         <v>43684</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="J6" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="18">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18" t="s">
+      <c r="F7" s="17"/>
+      <c r="G7" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="20">
         <v>43684</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="J7" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="17" t="s">
         <v>61</v>
       </c>
     </row>
@@ -964,28 +964,28 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.26953125" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="48.08984375" customWidth="1"/>
-    <col min="4" max="5" width="15.90625" customWidth="1"/>
-    <col min="6" max="6" width="16.26953125" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" customWidth="1"/>
+    <col min="4" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:7" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-    </row>
-    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>7</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>9</v>
       </c>

</xml_diff>